<commit_message>
Working in progress: creating columns
</commit_message>
<xml_diff>
--- a/testdata/test_survey_test_data_2.xlsx
+++ b/testdata/test_survey_test_data_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0abb2bdfbe6dd6ae/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0abb2bdfbe6dd6ae/Documents/Github/team-58/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9232ADB6-9052-43E1-B837-3CC4E176C0DE}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40C577E9-23C6-4454-9A09-AC480957E8BE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{FF970D1A-0688-4BC7-84FC-C8B3384AC219}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>ASUrite ID</t>
   </si>
@@ -655,7 +655,7 @@
   <dimension ref="A1:BN21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -870,6 +870,30 @@
       <c r="B2" t="s">
         <v>68</v>
       </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Adjusted number of participants to 25
</commit_message>
<xml_diff>
--- a/testdata/test_survey_test_data_2.xlsx
+++ b/testdata/test_survey_test_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0abb2bdfbe6dd6ae/Documents/Github/team-58/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40C577E9-23C6-4454-9A09-AC480957E8BE}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84308FBA-C0E7-407C-B1CC-2794313FDD16}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{FF970D1A-0688-4BC7-84FC-C8B3384AC219}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t>ASUrite ID</t>
   </si>
@@ -294,6 +294,18 @@
   </si>
   <si>
     <t>A20</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>A24</t>
   </si>
 </sst>
 </file>
@@ -652,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDD676D-6D2C-418F-B9E7-7350CD4F8264}">
-  <dimension ref="A1:BN21"/>
+  <dimension ref="A1:BN25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -880,10 +892,7 @@
         <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
         <v>70</v>
@@ -1044,6 +1053,38 @@
         <v>86</v>
       </c>
       <c r="B21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make some progress on creating test data with the first 3 students
</commit_message>
<xml_diff>
--- a/testdata/test_survey_test_data_2.xlsx
+++ b/testdata/test_survey_test_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0abb2bdfbe6dd6ae/Documents/Github/team-58/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84308FBA-C0E7-407C-B1CC-2794313FDD16}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1253F177-FBCA-42D6-AF2D-A7358F043D3F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{FF970D1A-0688-4BC7-84FC-C8B3384AC219}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
   <si>
     <t>ASUrite ID</t>
   </si>
@@ -306,13 +306,16 @@
   </si>
   <si>
     <t>A24</t>
+  </si>
+  <si>
+    <t>A25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,13 +329,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -344,14 +359,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -664,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDD676D-6D2C-418F-B9E7-7350CD4F8264}">
-  <dimension ref="A1:BN25"/>
+  <dimension ref="A1:BN26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="BG50" sqref="BG50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -903,6 +921,30 @@
       <c r="J2" t="s">
         <v>76</v>
       </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BJ2" s="2"/>
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -911,6 +953,29 @@
       <c r="B3" t="s">
         <v>68</v>
       </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BL3" s="2"/>
+      <c r="BM3" s="2"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -919,6 +984,37 @@
       <c r="B4" t="s">
         <v>68</v>
       </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+      <c r="BD4" s="2"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1085,6 +1181,14 @@
         <v>90</v>
       </c>
       <c r="B25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make some progress on creating test data with the first 10 students
</commit_message>
<xml_diff>
--- a/testdata/test_survey_test_data_2.xlsx
+++ b/testdata/test_survey_test_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0abb2bdfbe6dd6ae/Documents/Github/team-58/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1253F177-FBCA-42D6-AF2D-A7358F043D3F}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBE21387-85FA-4DCB-ACBE-B90324E15A3D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{FF970D1A-0688-4BC7-84FC-C8B3384AC219}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
   <si>
     <t>ASUrite ID</t>
   </si>
@@ -685,7 +685,7 @@
   <dimension ref="A1:BN26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="BG50" sqref="BG50"/>
+      <selection activeCell="BC23" sqref="BC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -954,7 +954,7 @@
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
         <v>74</v>
@@ -1023,6 +1023,37 @@
       <c r="B5" t="s">
         <v>68</v>
       </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s">
+        <v>71</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="BC5" s="2"/>
+      <c r="BD5" s="2"/>
+      <c r="BE5" s="2"/>
+      <c r="BK5" s="2"/>
+      <c r="BL5" s="2"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -1039,6 +1070,42 @@
       <c r="B7" t="s">
         <v>68</v>
       </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="2"/>
+      <c r="BI7" s="2"/>
+      <c r="BJ7" s="2"/>
+      <c r="BK7" s="2"/>
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1047,6 +1114,44 @@
       <c r="B8" t="s">
         <v>68</v>
       </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="BC8" s="2"/>
+      <c r="BD8" s="2"/>
+      <c r="BE8" s="2"/>
+      <c r="BF8" s="2"/>
+      <c r="BI8" s="2"/>
+      <c r="BJ8" s="2"/>
+      <c r="BK8" s="2"/>
+      <c r="BL8" s="2"/>
     </row>
     <row r="9" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1055,6 +1160,55 @@
       <c r="B9" t="s">
         <v>68</v>
       </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
+      <c r="BD9" s="2"/>
+      <c r="BE9" s="2"/>
+      <c r="BF9" s="2"/>
+      <c r="BJ9" s="2"/>
+      <c r="BK9" s="2"/>
+      <c r="BL9" s="2"/>
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1063,6 +1217,42 @@
       <c r="B10" t="s">
         <v>68</v>
       </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+      <c r="BC10" s="2"/>
+      <c r="BD10" s="2"/>
+      <c r="BE10" s="2"/>
+      <c r="BK10" s="2"/>
+      <c r="BL10" s="2"/>
+      <c r="BM10" s="2"/>
     </row>
     <row r="11" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1071,6 +1261,37 @@
       <c r="B11" t="s">
         <v>68</v>
       </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" t="s">
+        <v>88</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+      <c r="BD11" s="2"/>
+      <c r="BE11" s="2"/>
+      <c r="BF11" s="2"/>
+      <c r="BI11" s="2"/>
+      <c r="BJ11" s="2"/>
+      <c r="BK11" s="2"/>
+      <c r="BL11" s="2"/>
+      <c r="BM11" s="2"/>
+      <c r="BN11" s="2"/>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Make some progress on creating test data with the first 20 students
</commit_message>
<xml_diff>
--- a/testdata/test_survey_test_data_2.xlsx
+++ b/testdata/test_survey_test_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0abb2bdfbe6dd6ae/Documents/Github/team-58/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBE21387-85FA-4DCB-ACBE-B90324E15A3D}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60A63018-CE69-4C89-A703-5D345EB0A413}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{FF970D1A-0688-4BC7-84FC-C8B3384AC219}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="92">
   <si>
     <t>ASUrite ID</t>
   </si>
@@ -315,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,8 +336,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +359,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3ECD35"/>
+        <bgColor rgb="FF3ECD35"/>
       </patternFill>
     </fill>
   </fills>
@@ -363,10 +381,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -685,7 +705,7 @@
   <dimension ref="A1:BN26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="BC23" sqref="BC23"/>
+      <selection activeCell="BE40" sqref="BE40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,20 +941,20 @@
       <c r="J2" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="3"/>
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
@@ -962,14 +982,14 @@
       <c r="H3" t="s">
         <v>86</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3"/>
       <c r="AV3" s="2"/>
       <c r="AW3" s="2"/>
       <c r="BD3" s="2"/>
@@ -999,15 +1019,15 @@
       <c r="I4" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
       <c r="AS4" s="2"/>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
@@ -1035,15 +1055,15 @@
       <c r="I5" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2"/>
-      <c r="AN5" s="2"/>
-      <c r="AO5" s="2"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
       <c r="AS5" s="2"/>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
@@ -1062,6 +1082,36 @@
       <c r="B6" t="s">
         <v>68</v>
       </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+      <c r="BD6" s="2"/>
+      <c r="BE6" s="2"/>
+      <c r="BF6" s="2"/>
+      <c r="BJ6" s="2"/>
+      <c r="BK6" s="2"/>
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1085,18 +1135,18 @@
       <c r="I7" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="2"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
@@ -1132,15 +1182,15 @@
       <c r="I8" t="s">
         <v>81</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
       <c r="AV8" s="2"/>
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
@@ -1178,24 +1228,24 @@
       <c r="J9" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2"/>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="2"/>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="2"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
       <c r="AV9" s="2"/>
@@ -1232,18 +1282,18 @@
       <c r="J10" t="s">
         <v>67</v>
       </c>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2"/>
-      <c r="AM10" s="2"/>
-      <c r="AN10" s="2"/>
-      <c r="AO10" s="2"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
       <c r="AU10" s="2"/>
       <c r="AV10" s="2"/>
       <c r="AW10" s="2"/>
@@ -1270,14 +1320,14 @@
       <c r="I11" t="s">
         <v>88</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-      <c r="AK11" s="2"/>
-      <c r="AL11" s="2"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
       <c r="AS11" s="2"/>
       <c r="AT11" s="2"/>
       <c r="BA11" s="2"/>
@@ -1300,6 +1350,46 @@
       <c r="B12" t="s">
         <v>68</v>
       </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="2"/>
+      <c r="BG12" s="2"/>
+      <c r="BH12" s="2"/>
+      <c r="BI12" s="2"/>
+      <c r="BJ12" s="2"/>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1308,6 +1398,36 @@
       <c r="B13" t="s">
         <v>68</v>
       </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="BD13" s="2"/>
+      <c r="BE13" s="2"/>
+      <c r="BF13" s="2"/>
+      <c r="BJ13" s="2"/>
+      <c r="BK13" s="2"/>
+      <c r="BL13" s="2"/>
+      <c r="BM13" s="2"/>
+      <c r="BN13" s="2"/>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1316,6 +1436,52 @@
       <c r="B14" t="s">
         <v>68</v>
       </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" t="s">
+        <v>82</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2"/>
+      <c r="BE14" s="2"/>
+      <c r="BF14" s="2"/>
+      <c r="BI14" s="2"/>
+      <c r="BJ14" s="2"/>
+      <c r="BM14" s="2"/>
+      <c r="BN14" s="2"/>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1324,6 +1490,44 @@
       <c r="B15" t="s">
         <v>68</v>
       </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" t="s">
+        <v>75</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="2"/>
+      <c r="BD15" s="2"/>
+      <c r="BJ15" s="2"/>
+      <c r="BK15" s="2"/>
+      <c r="BL15" s="2"/>
+      <c r="BM15" s="2"/>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1332,48 +1536,229 @@
       <c r="B16" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" t="s">
+        <v>80</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AV16" s="2"/>
+      <c r="AW16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2"/>
+      <c r="BD16" s="2"/>
+      <c r="BE16" s="2"/>
+      <c r="BF16" s="2"/>
+      <c r="BG16" s="2"/>
+      <c r="BK16" s="2"/>
+      <c r="BL16" s="2"/>
+      <c r="BM16" s="2"/>
+      <c r="BN16" s="2"/>
+    </row>
+    <row r="17" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>82</v>
       </c>
       <c r="B17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AT17" s="2"/>
+      <c r="AU17" s="2"/>
+      <c r="AV17" s="2"/>
+      <c r="AW17" s="2"/>
+      <c r="AX17" s="2"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="2"/>
+      <c r="BD17" s="2"/>
+      <c r="BE17" s="2"/>
+      <c r="BF17" s="2"/>
+      <c r="BJ17" s="2"/>
+      <c r="BK17" s="2"/>
+      <c r="BL17" s="2"/>
+      <c r="BM17" s="2"/>
+      <c r="BN17" s="2"/>
+    </row>
+    <row r="18" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>83</v>
       </c>
       <c r="B18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>82</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="2"/>
+      <c r="AP18" s="2"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="2"/>
+      <c r="AZ18" s="2"/>
+      <c r="BA18" s="2"/>
+      <c r="BF18" s="2"/>
+      <c r="BG18" s="2"/>
+      <c r="BH18" s="2"/>
+      <c r="BI18" s="2"/>
+      <c r="BN18" s="2"/>
+    </row>
+    <row r="19" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>84</v>
       </c>
       <c r="B19" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
+      <c r="AR19" s="2"/>
+      <c r="AS19" s="2"/>
+      <c r="AT19" s="2"/>
+      <c r="AZ19" s="2"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BH19" s="2"/>
+      <c r="BI19" s="2"/>
+      <c r="BJ19" s="2"/>
+    </row>
+    <row r="20" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>85</v>
       </c>
       <c r="B20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" t="s">
+        <v>80</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="2"/>
+      <c r="AK20" s="2"/>
+      <c r="AQ20" s="2"/>
+      <c r="AR20" s="2"/>
+      <c r="AS20" s="2"/>
+      <c r="AY20" s="2"/>
+      <c r="AZ20" s="2"/>
+      <c r="BA20" s="2"/>
+      <c r="BG20" s="2"/>
+      <c r="BH20" s="2"/>
+      <c r="BI20" s="2"/>
+    </row>
+    <row r="21" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>86</v>
       </c>
       <c r="B21" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1381,7 +1766,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1389,7 +1774,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1397,15 +1782,16 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>90</v>
       </c>
       <c r="B25" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -1414,6 +1800,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Making edits to data WIP
</commit_message>
<xml_diff>
--- a/testdata/test_survey_test_data_2.xlsx
+++ b/testdata/test_survey_test_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0abb2bdfbe6dd6ae/Documents/Github/team-58/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="397" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60A63018-CE69-4C89-A703-5D345EB0A413}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F57B74A2-6603-44A9-B46E-CF40B846ED8E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{FF970D1A-0688-4BC7-84FC-C8B3384AC219}"/>
   </bookViews>
@@ -381,12 +381,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -704,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDD676D-6D2C-418F-B9E7-7350CD4F8264}">
   <dimension ref="A1:BN26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="BE40" sqref="BE40"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="BI21" sqref="BI21:BM21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1757,6 +1756,41 @@
       <c r="C21" t="s">
         <v>87</v>
       </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+      <c r="BD21" s="2"/>
+      <c r="BE21" s="2"/>
+      <c r="BI21" s="2"/>
+      <c r="BJ21" s="2"/>
+      <c r="BK21" s="2"/>
+      <c r="BL21" s="2"/>
+      <c r="BM21" s="2"/>
     </row>
     <row r="22" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -1789,7 +1823,6 @@
       <c r="B25" t="s">
         <v>68</v>
       </c>
-      <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
Making final additions to test data 2
</commit_message>
<xml_diff>
--- a/testdata/test_survey_test_data_2.xlsx
+++ b/testdata/test_survey_test_data_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0abb2bdfbe6dd6ae/Documents/Github/team-58/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F57B74A2-6603-44A9-B46E-CF40B846ED8E}"/>
+  <xr:revisionPtr revIDLastSave="470" documentId="8_{0E983EF1-642A-4EE6-A043-AEDB8D287A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F480D4D-867C-4D7E-8AEA-1041914CDD55}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{FF970D1A-0688-4BC7-84FC-C8B3384AC219}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="92">
   <si>
     <t>ASUrite ID</t>
   </si>
@@ -315,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,13 +330,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -349,17 +342,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -377,18 +365,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -703,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDD676D-6D2C-418F-B9E7-7350CD4F8264}">
   <dimension ref="A1:BN26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="BI21" sqref="BI21:BM21"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,20 +925,20 @@
       <c r="J2" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
       <c r="AT2" s="2"/>
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
@@ -981,14 +966,14 @@
       <c r="H3" t="s">
         <v>86</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
-      <c r="AN3" s="3"/>
-      <c r="AO3" s="3"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
       <c r="AV3" s="2"/>
       <c r="AW3" s="2"/>
       <c r="BD3" s="2"/>
@@ -1018,15 +1003,15 @@
       <c r="I4" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AK4" s="3"/>
-      <c r="AL4" s="3"/>
-      <c r="AM4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
       <c r="AS4" s="2"/>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
@@ -1054,15 +1039,15 @@
       <c r="I5" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AN5" s="3"/>
-      <c r="AO5" s="3"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
       <c r="AS5" s="2"/>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
@@ -1087,18 +1072,18 @@
       <c r="D6" t="s">
         <v>91</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="3"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
       <c r="AV6" s="2"/>
@@ -1134,18 +1119,18 @@
       <c r="I7" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
@@ -1181,15 +1166,15 @@
       <c r="I8" t="s">
         <v>81</v>
       </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
       <c r="AV8" s="2"/>
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
@@ -1227,24 +1212,24 @@
       <c r="J9" t="s">
         <v>76</v>
       </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AL9" s="3"/>
-      <c r="AM9" s="3"/>
-      <c r="AN9" s="3"/>
-      <c r="AO9" s="3"/>
-      <c r="AP9" s="3"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
       <c r="AV9" s="2"/>
@@ -1281,18 +1266,18 @@
       <c r="J10" t="s">
         <v>67</v>
       </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
       <c r="AU10" s="2"/>
       <c r="AV10" s="2"/>
       <c r="AW10" s="2"/>
@@ -1319,14 +1304,14 @@
       <c r="I11" t="s">
         <v>88</v>
       </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AK11" s="3"/>
-      <c r="AL11" s="3"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
       <c r="AS11" s="2"/>
       <c r="AT11" s="2"/>
       <c r="BA11" s="2"/>
@@ -1361,18 +1346,18 @@
       <c r="I12" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
@@ -1403,13 +1388,13 @@
       <c r="H13" t="s">
         <v>91</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
@@ -1453,14 +1438,14 @@
       <c r="I14" t="s">
         <v>82</v>
       </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
       <c r="AG14" s="2"/>
@@ -1504,10 +1489,10 @@
       <c r="J15" t="s">
         <v>75</v>
       </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
@@ -1547,9 +1532,9 @@
       <c r="I16" t="s">
         <v>80</v>
       </c>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
@@ -1582,10 +1567,10 @@
       <c r="B17" t="s">
         <v>68</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
@@ -1632,9 +1617,9 @@
       <c r="I18" t="s">
         <v>82</v>
       </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
@@ -1686,9 +1671,9 @@
       <c r="J19" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
@@ -1799,6 +1784,52 @@
       <c r="B22" t="s">
         <v>68</v>
       </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" t="s">
+        <v>77</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" t="s">
+        <v>91</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="BA22" s="2"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="2"/>
+      <c r="BD22" s="2"/>
+      <c r="BI22" s="2"/>
+      <c r="BJ22" s="2"/>
+      <c r="BK22" s="2"/>
+      <c r="BL22" s="2"/>
     </row>
     <row r="23" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -1807,6 +1838,55 @@
       <c r="B23" t="s">
         <v>68</v>
       </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="2"/>
+      <c r="AS23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23" s="2"/>
+      <c r="AZ23" s="2"/>
+      <c r="BA23" s="2"/>
+      <c r="BF23" s="2"/>
+      <c r="BG23" s="2"/>
+      <c r="BH23" s="2"/>
+      <c r="BI23" s="2"/>
+      <c r="BN23" s="2"/>
     </row>
     <row r="24" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -1815,6 +1895,45 @@
       <c r="B24" t="s">
         <v>68</v>
       </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" t="s">
+        <v>74</v>
+      </c>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+      <c r="BC24" s="2"/>
+      <c r="BD24" s="2"/>
+      <c r="BE24" s="2"/>
+      <c r="BJ24" s="2"/>
+      <c r="BK24" s="2"/>
+      <c r="BL24" s="2"/>
+      <c r="BM24" s="2"/>
     </row>
     <row r="25" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -1823,6 +1942,59 @@
       <c r="B25" t="s">
         <v>68</v>
       </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" t="s">
+        <v>84</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+      <c r="AP25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+      <c r="BD25" s="2"/>
+      <c r="BE25" s="2"/>
+      <c r="BF25" s="2"/>
+      <c r="BK25" s="2"/>
+      <c r="BL25" s="2"/>
+      <c r="BM25" s="2"/>
     </row>
     <row r="26" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -1833,7 +2005,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>